<commit_message>
Update median of clusters (normbysoul) no mundist-f.xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/median of clusters (normbysoul) no mundist-f.xlsx
+++ b/migforecasting/clustering/median of clusters (normbysoul) no mundist-f.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>clust</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>migprop</t>
+  </si>
+  <si>
+    <t>сельхоз (посев)</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>промыш</t>
+  </si>
+  <si>
+    <t>сельхоз (скот и посев)</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -170,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -186,6 +201,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,16 +507,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -507,9 +525,10 @@
     <col min="12" max="16" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.42578125" customWidth="1"/>
     <col min="18" max="18" width="14.42578125" customWidth="1"/>
+    <col min="20" max="20" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +586,11 @@
       <c r="S1" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="T1" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -627,8 +649,11 @@
         <f>B2/C2</f>
         <v>-2.1058389169971289E-3</v>
       </c>
+      <c r="T2" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -687,8 +712,11 @@
         <f t="shared" ref="S3:S7" si="0">B3/C3</f>
         <v>2.2546007947467828E-4</v>
       </c>
+      <c r="T3" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -747,8 +775,11 @@
         <f t="shared" si="0"/>
         <v>-4.1298459079000139E-3</v>
       </c>
+      <c r="T4" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -807,8 +838,11 @@
         <f t="shared" si="0"/>
         <v>-3.3845242628082954E-3</v>
       </c>
+      <c r="T5" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -867,8 +901,11 @@
         <f t="shared" si="0"/>
         <v>-1.216106657057923E-3</v>
       </c>
+      <c r="T6" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -927,9 +964,24 @@
         <f t="shared" si="0"/>
         <v>-1.1729691876750687E-3</v>
       </c>
+      <c r="T7" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C7">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -941,7 +993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="E2:E7">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -953,7 +1005,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E7">
+  <conditionalFormatting sqref="F2:F7">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -965,7 +1017,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F7">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -977,7 +1029,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -989,7 +1041,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -1001,7 +1053,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1013,7 +1065,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="K2:K7">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -1025,7 +1077,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K7">
+  <conditionalFormatting sqref="L2:L7">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1037,7 +1089,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L7">
+  <conditionalFormatting sqref="M2:M7">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1049,7 +1101,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M7">
+  <conditionalFormatting sqref="N2:N7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1061,7 +1113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N7">
+  <conditionalFormatting sqref="O2:O7">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1073,7 +1125,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O7">
+  <conditionalFormatting sqref="P2:P7">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1085,7 +1137,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P7">
+  <conditionalFormatting sqref="Q2:Q7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1097,7 +1149,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q7">
+  <conditionalFormatting sqref="R2:R7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1109,7 +1161,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R7">
+  <conditionalFormatting sqref="S2:S7">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1121,7 +1173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S7">
+  <conditionalFormatting sqref="B2:B7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>